<commit_message>
Qgis Processing works now
</commit_message>
<xml_diff>
--- a/countries.xlsx
+++ b/countries.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\PycharmProjects\pythonProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\martin\PycharmProjects\HeatMapMaker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{493EBF58-22B5-4727-BFB5-A18D8C292BF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E4AD556-E849-4969-AB7B-83F622215470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88131578-78CB-433C-B784-66E47A35BA83}"/>
   </bookViews>
@@ -1976,13 +1976,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E85A6051-971E-449C-91C3-F94872696AE6}">
   <dimension ref="A1:O241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="A221" workbookViewId="0">
+      <selection activeCell="A240" sqref="A240"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>528</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>526</v>
       </c>
@@ -2010,7 +2010,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>524</v>
       </c>
@@ -2021,7 +2021,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>522</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>520</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>518</v>
       </c>
@@ -2060,7 +2060,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>516</v>
       </c>
@@ -2071,7 +2071,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>514</v>
       </c>
@@ -2088,7 +2088,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>512</v>
       </c>
@@ -2099,7 +2099,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>510</v>
       </c>
@@ -2122,7 +2122,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>507</v>
       </c>
@@ -2133,7 +2133,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>505</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>503</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>501</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>499</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>497</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>495</v>
       </c>
@@ -2199,7 +2199,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>493</v>
       </c>
@@ -2210,7 +2210,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>491</v>
       </c>
@@ -2221,7 +2221,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>489</v>
       </c>
@@ -2232,7 +2232,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>487</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>485</v>
       </c>
@@ -2254,7 +2254,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>483</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>481</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>479</v>
       </c>
@@ -2287,7 +2287,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>477</v>
       </c>
@@ -2298,7 +2298,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>475</v>
       </c>
@@ -2309,7 +2309,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>473</v>
       </c>
@@ -2332,7 +2332,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>470</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>468</v>
       </c>
@@ -2360,7 +2360,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>466</v>
       </c>
@@ -2371,7 +2371,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>464</v>
       </c>
@@ -2400,7 +2400,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>460</v>
       </c>
@@ -2423,7 +2423,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>457</v>
       </c>
@@ -2440,7 +2440,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>454</v>
       </c>
@@ -2451,7 +2451,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>452</v>
       </c>
@@ -2468,7 +2468,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>449</v>
       </c>
@@ -2479,7 +2479,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>447</v>
       </c>
@@ -2490,7 +2490,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>445</v>
       </c>
@@ -2501,7 +2501,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>443</v>
       </c>
@@ -2512,7 +2512,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>441</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>438</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>436</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>433</v>
       </c>
@@ -2580,7 +2580,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>431</v>
       </c>
@@ -2591,7 +2591,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>429</v>
       </c>
@@ -2602,7 +2602,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>427</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>425</v>
       </c>
@@ -2636,7 +2636,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>423</v>
       </c>
@@ -2647,7 +2647,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>421</v>
       </c>
@@ -2658,7 +2658,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>419</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>418</v>
       </c>
@@ -2722,7 +2722,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>414</v>
       </c>
@@ -2739,7 +2739,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>412</v>
       </c>
@@ -2756,7 +2756,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>409</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>406</v>
       </c>
@@ -2784,7 +2784,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>404</v>
       </c>
@@ -2795,7 +2795,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>402</v>
       </c>
@@ -2806,7 +2806,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>400</v>
       </c>
@@ -2823,7 +2823,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>398</v>
       </c>
@@ -2834,7 +2834,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>396</v>
       </c>
@@ -2845,7 +2845,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>394</v>
       </c>
@@ -2856,7 +2856,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>392</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>389</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>387</v>
       </c>
@@ -2895,7 +2895,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>385</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>382</v>
       </c>
@@ -2929,7 +2929,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>380</v>
       </c>
@@ -2940,7 +2940,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>378</v>
       </c>
@@ -2951,7 +2951,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>376</v>
       </c>
@@ -2962,7 +2962,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>374</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>372</v>
       </c>
@@ -2996,7 +2996,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>370</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>368</v>
       </c>
@@ -3018,7 +3018,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>366</v>
       </c>
@@ -3029,7 +3029,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>364</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>362</v>
       </c>
@@ -3063,7 +3063,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>360</v>
       </c>
@@ -3086,7 +3086,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>356</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>354</v>
       </c>
@@ -3108,7 +3108,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>352</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>351</v>
       </c>
@@ -3130,7 +3130,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>349</v>
       </c>
@@ -3141,7 +3141,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>347</v>
       </c>
@@ -3152,7 +3152,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>345</v>
       </c>
@@ -3163,7 +3163,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>343</v>
       </c>
@@ -3174,7 +3174,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>341</v>
       </c>
@@ -3185,7 +3185,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>339</v>
       </c>
@@ -3196,7 +3196,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>337</v>
       </c>
@@ -3207,7 +3207,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>335</v>
       </c>
@@ -3218,7 +3218,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>333</v>
       </c>
@@ -3229,7 +3229,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>331</v>
       </c>
@@ -3240,7 +3240,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>330</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>328</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>326</v>
       </c>
@@ -3273,7 +3273,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>324</v>
       </c>
@@ -3308,7 +3308,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>321</v>
       </c>
@@ -3319,7 +3319,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>319</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>317</v>
       </c>
@@ -3341,7 +3341,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>315</v>
       </c>
@@ -3352,7 +3352,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>313</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>311</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>309</v>
       </c>
@@ -3385,7 +3385,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>307</v>
       </c>
@@ -3396,7 +3396,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>305</v>
       </c>
@@ -3407,7 +3407,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>303</v>
       </c>
@@ -3430,7 +3430,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>300</v>
       </c>
@@ -3441,7 +3441,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>298</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>296</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>294</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>292</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>290</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>288</v>
       </c>
@@ -3507,7 +3507,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>286</v>
       </c>
@@ -3518,7 +3518,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>284</v>
       </c>
@@ -3529,7 +3529,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>282</v>
       </c>
@@ -3540,7 +3540,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>280</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>278</v>
       </c>
@@ -3562,7 +3562,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>276</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>274</v>
       </c>
@@ -3584,7 +3584,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>272</v>
       </c>
@@ -3595,7 +3595,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>270</v>
       </c>
@@ -3606,7 +3606,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>268</v>
       </c>
@@ -3617,7 +3617,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>266</v>
       </c>
@@ -3628,7 +3628,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>264</v>
       </c>
@@ -3639,7 +3639,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>262</v>
       </c>
@@ -3650,7 +3650,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>260</v>
       </c>
@@ -3661,7 +3661,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>258</v>
       </c>
@@ -3672,7 +3672,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>256</v>
       </c>
@@ -3683,7 +3683,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>254</v>
       </c>
@@ -3694,7 +3694,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>252</v>
       </c>
@@ -3705,7 +3705,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>250</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>248</v>
       </c>
@@ -3727,7 +3727,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>246</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>244</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>242</v>
       </c>
@@ -3766,7 +3766,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>240</v>
       </c>
@@ -3777,7 +3777,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>238</v>
       </c>
@@ -3788,7 +3788,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>236</v>
       </c>
@@ -3799,7 +3799,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>234</v>
       </c>
@@ -3810,7 +3810,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>232</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>228</v>
       </c>
@@ -3850,7 +3850,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>226</v>
       </c>
@@ -3861,7 +3861,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>224</v>
       </c>
@@ -3872,7 +3872,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>222</v>
       </c>
@@ -3883,7 +3883,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>220</v>
       </c>
@@ -3894,7 +3894,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>218</v>
       </c>
@@ -3905,7 +3905,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>216</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>214</v>
       </c>
@@ -3927,7 +3927,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>212</v>
       </c>
@@ -3938,7 +3938,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>210</v>
       </c>
@@ -3949,7 +3949,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>208</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>206</v>
       </c>
@@ -3971,7 +3971,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>205</v>
       </c>
@@ -3988,7 +3988,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>202</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>200</v>
       </c>
@@ -4022,7 +4022,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>198</v>
       </c>
@@ -4033,7 +4033,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>196</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>194</v>
       </c>
@@ -4055,7 +4055,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>192</v>
       </c>
@@ -4066,7 +4066,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>190</v>
       </c>
@@ -4083,7 +4083,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>187</v>
       </c>
@@ -4100,7 +4100,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="163" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>185</v>
       </c>
@@ -4123,7 +4123,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="164" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>182</v>
       </c>
@@ -4134,7 +4134,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="165" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>180</v>
       </c>
@@ -4145,7 +4145,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>178</v>
       </c>
@@ -4156,7 +4156,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>176</v>
       </c>
@@ -4167,7 +4167,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="168" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>174</v>
       </c>
@@ -4178,7 +4178,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="169" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>172</v>
       </c>
@@ -4189,7 +4189,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>170</v>
       </c>
@@ -4212,7 +4212,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="171" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>166</v>
       </c>
@@ -4223,7 +4223,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>164</v>
       </c>
@@ -4234,7 +4234,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="173" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>162</v>
       </c>
@@ -4245,7 +4245,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="174" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>160</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="175" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>158</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="176" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>156</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>154</v>
       </c>
@@ -4301,7 +4301,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>151</v>
       </c>
@@ -4312,7 +4312,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>149</v>
       </c>
@@ -4323,7 +4323,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>147</v>
       </c>
@@ -4334,7 +4334,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>145</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>142</v>
       </c>
@@ -4362,7 +4362,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>140</v>
       </c>
@@ -4379,7 +4379,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>138</v>
       </c>
@@ -4408,7 +4408,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>135</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>132</v>
       </c>
@@ -4472,7 +4472,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>128</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>126</v>
       </c>
@@ -4500,7 +4500,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>123</v>
       </c>
@@ -4517,7 +4517,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>120</v>
       </c>
@@ -4546,7 +4546,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>116</v>
       </c>
@@ -4563,7 +4563,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>113</v>
       </c>
@@ -4574,7 +4574,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="193" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>111</v>
       </c>
@@ -4585,7 +4585,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="194" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>109</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="195" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>107</v>
       </c>
@@ -4613,7 +4613,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="196" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>104</v>
       </c>
@@ -4624,7 +4624,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="197" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>102</v>
       </c>
@@ -4635,7 +4635,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="198" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>100</v>
       </c>
@@ -4646,7 +4646,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="199" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>98</v>
       </c>
@@ -4663,7 +4663,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="200" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>96</v>
       </c>
@@ -4674,7 +4674,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="201" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>94</v>
       </c>
@@ -4691,7 +4691,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="202" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>92</v>
       </c>
@@ -4738,7 +4738,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="203" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>88</v>
       </c>
@@ -4755,7 +4755,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="204" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>85</v>
       </c>
@@ -4766,7 +4766,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="205" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>83</v>
       </c>
@@ -4783,7 +4783,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="206" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>80</v>
       </c>
@@ -4794,7 +4794,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="207" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>78</v>
       </c>
@@ -4805,7 +4805,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="208" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>76</v>
       </c>
@@ -4834,7 +4834,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="209" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>72</v>
       </c>
@@ -4845,7 +4845,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="210" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>70</v>
       </c>
@@ -4856,7 +4856,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="211" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>68</v>
       </c>
@@ -4867,7 +4867,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="212" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>66</v>
       </c>
@@ -4878,7 +4878,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="213" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>64</v>
       </c>
@@ -4889,7 +4889,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="214" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>62</v>
       </c>
@@ -4900,7 +4900,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="215" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>60</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="216" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>58</v>
       </c>
@@ -4922,7 +4922,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="217" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>56</v>
       </c>
@@ -4933,7 +4933,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="218" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>54</v>
       </c>
@@ -4944,7 +4944,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="219" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>52</v>
       </c>
@@ -4955,7 +4955,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="220" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>50</v>
       </c>
@@ -4966,7 +4966,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="221" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>48</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="222" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>45</v>
       </c>
@@ -5000,7 +5000,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="223" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>43</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="224" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>41</v>
       </c>
@@ -5022,7 +5022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>39</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>34</v>
       </c>
@@ -5062,7 +5062,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>32</v>
       </c>
@@ -5073,7 +5073,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>30</v>
       </c>
@@ -5084,7 +5084,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>28</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>25</v>
       </c>
@@ -5124,7 +5124,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>23</v>
       </c>
@@ -5141,7 +5141,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>20</v>
       </c>
@@ -5152,7 +5152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>18</v>
       </c>
@@ -5163,7 +5163,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>16</v>
       </c>
@@ -5174,7 +5174,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>14</v>
       </c>
@@ -5185,7 +5185,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>12</v>
       </c>
@@ -5196,7 +5196,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>10</v>
       </c>
@@ -5207,7 +5207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>8</v>
       </c>
@@ -5224,7 +5224,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>5</v>
       </c>
@@ -5235,7 +5235,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>3</v>
       </c>
@@ -5246,7 +5246,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="241" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>1</v>
       </c>

</xml_diff>